<commit_message>
Pluto dependencies bug fix
</commit_message>
<xml_diff>
--- a/NoCode_Interface/Gundersen_4_stream.xlsx
+++ b/NoCode_Interface/Gundersen_4_stream.xlsx
@@ -189,7 +189,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -322,10 +322,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>250</v>
+        <v>380</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>249</v>
+        <v>379</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>1</v>

</xml_diff>